<commit_message>
Add ability content loading
</commit_message>
<xml_diff>
--- a/content/content.xlsx
+++ b/content/content.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Urbanyeti\source\repos\go-hero-game\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29D8A564-C33B-45F9-A24F-4B99715405F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ED54A4-3DB3-44E3-8487-E19221B503AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="690" windowWidth="17415" windowHeight="10785" activeTab="2" xr2:uid="{7C3BB7F5-07B4-41EB-913E-FADE0D43664E}"/>
+    <workbookView xWindow="3030" yWindow="1875" windowWidth="17415" windowHeight="10785" activeTab="3" xr2:uid="{7C3BB7F5-07B4-41EB-913E-FADE0D43664E}"/>
   </bookViews>
   <sheets>
     <sheet name="monsters" sheetId="3" r:id="rId1"/>
     <sheet name="weapons" sheetId="1" r:id="rId2"/>
     <sheet name="armor" sheetId="2" r:id="rId3"/>
+    <sheet name="attacks" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>id</t>
   </si>
@@ -189,6 +190,39 @@
   </si>
   <si>
     <t>character,monster,troll</t>
+  </si>
+  <si>
+    <t>attack-tongue1</t>
+  </si>
+  <si>
+    <t>attack-spit1</t>
+  </si>
+  <si>
+    <t>Claw Attack</t>
+  </si>
+  <si>
+    <t>Tongue Smack</t>
+  </si>
+  <si>
+    <t>Acid Spit</t>
+  </si>
+  <si>
+    <t>swipe{!s} at {t} with their sharp claws</t>
+  </si>
+  <si>
+    <t>smacks{!s} {t} with their tongue</t>
+  </si>
+  <si>
+    <t>spit{!s} acid at {t}</t>
+  </si>
+  <si>
+    <t>ability,action,attack,melee,physical</t>
+  </si>
+  <si>
+    <t>ability,action,attack,ranged,physical</t>
+  </si>
+  <si>
+    <t>ability,action,attack,ranged,acid</t>
   </si>
 </sst>
 </file>
@@ -546,7 +580,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +755,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G1" sqref="G1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE418EE-3E84-415B-9A39-72CC9D1EF287}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,4 +1002,120 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94728EEE-FF30-4BD7-BDAC-4731EF3C31CF}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add multiple monster encounters
</commit_message>
<xml_diff>
--- a/content/content.xlsx
+++ b/content/content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Urbanyeti\source\repos\go-hero-game\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ED54A4-3DB3-44E3-8487-E19221B503AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FA0030-0DB2-40C0-81D8-BC78EA4E748B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="1875" windowWidth="17415" windowHeight="10785" activeTab="3" xr2:uid="{7C3BB7F5-07B4-41EB-913E-FADE0D43664E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7C3BB7F5-07B4-41EB-913E-FADE0D43664E}"/>
   </bookViews>
   <sheets>
     <sheet name="monsters" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
   <si>
     <t>id</t>
   </si>
@@ -223,6 +223,63 @@
   </si>
   <si>
     <t>ability,action,attack,ranged,acid</t>
+  </si>
+  <si>
+    <t>item-armor2</t>
+  </si>
+  <si>
+    <t>Fine Leather Armor</t>
+  </si>
+  <si>
+    <t>fine set of leather armor{s}</t>
+  </si>
+  <si>
+    <t>item-boots2</t>
+  </si>
+  <si>
+    <t>Fine Boots</t>
+  </si>
+  <si>
+    <t>pair{s} of fine boots</t>
+  </si>
+  <si>
+    <t>item-sword2</t>
+  </si>
+  <si>
+    <t>Fine Sword</t>
+  </si>
+  <si>
+    <t>fine steel sword{s}</t>
+  </si>
+  <si>
+    <t>Expert Club</t>
+  </si>
+  <si>
+    <t>expertly-crafted club{s}</t>
+  </si>
+  <si>
+    <t>monster-giant</t>
+  </si>
+  <si>
+    <t>Giant</t>
+  </si>
+  <si>
+    <t>giant{s}</t>
+  </si>
+  <si>
+    <t>character,monster,giant</t>
+  </si>
+  <si>
+    <t>item-club2</t>
+  </si>
+  <si>
+    <t>Stomp</t>
+  </si>
+  <si>
+    <t>destroy{!s} the ground with a fierce stomp</t>
+  </si>
+  <si>
+    <t>attack-stomp1</t>
   </si>
 </sst>
 </file>
@@ -577,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3326E12A-A157-4AB1-A1E4-856A6CC53F91}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,6 +802,44 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -752,10 +847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D618AAA0-9453-48F9-9738-30C41A067DA5}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,48 +955,98 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1">
         <v>2</v>
       </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>50</v>
-      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
+        <v>80</v>
+      </c>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G6" s="1">
         <v>5</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H6" s="1">
         <v>3</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J6" s="1">
         <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -911,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE418EE-3E84-415B-9A39-72CC9D1EF287}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,21 +1126,61 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="I3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="I5">
         <v>1</v>
       </c>
     </row>
@@ -1006,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94728EEE-FF30-4BD7-BDAC-4731EF3C31CF}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,6 +1300,29 @@
         <v>120</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>